<commit_message>
MockUp, Pflichtenheft und Arbeitszeit auf neustem Stand
</commit_message>
<xml_diff>
--- a/WorkingHours/WorkingHours.xlsx
+++ b/WorkingHours/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauls\Desktop\StaticSiteGenerator\WorkingHours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HTL_Leonding\3BHIF\SYP\StaticSiteGenerator\WorkingHours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402D9D82-DD24-4B6C-B7E6-BA5403712E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB26FE0-E678-415B-A7C0-6C12845EAB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PaulSchein" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Datum</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>2,25h</t>
+  </si>
+  <si>
+    <t>MockUp verbessert, Projektantrag, Projektauftrag und Pflichtenheft verbessert</t>
   </si>
 </sst>
 </file>
@@ -381,7 +384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+    <sheetView zoomScale="131" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7A4CFC-292D-4A68-9CB6-60BD2C7F66B3}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,6 +496,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45364</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Moved all Documents to docs folder and added ERD and UML Diagram
</commit_message>
<xml_diff>
--- a/WorkingHours/WorkingHours.xlsx
+++ b/WorkingHours/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\StaticSiteGenerator\WorkingHours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267F8ACE-3329-4FB9-B484-4C72AED1AEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7299D03B-4C16-4663-A161-EE65FA4759A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PaulSchein" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
     <t>Datum</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Arbeitspakete und Meilenstein Termine</t>
+  </si>
+  <si>
+    <t>2h 20min</t>
+  </si>
+  <si>
+    <t>Klassendiagramm und ERD erstellt</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +439,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45379</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -440,10 +457,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE7B43D-064A-4B82-8DF1-53FBF226FBF2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView tabSelected="1" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,6 +501,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45379</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -491,10 +519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7A4CFC-292D-4A68-9CB6-60BD2C7F66B3}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +574,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45379</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added workingHours and changed meilensteine date because of a holiday
</commit_message>
<xml_diff>
--- a/WorkingHours/WorkingHours.xlsx
+++ b/WorkingHours/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Github\StaticSiteGenerator\WorkingHours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pauls\Desktop\StaticSiteGenerator\WorkingHours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7B0D4F-D1A1-4CD4-B4A8-261B0CD4BF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051211FD-DD8F-4125-8820-D177E657C006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PaulSchein" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>Datum</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Klassendiagramm und ERD bearbeitet und Projekt Setup</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Themes Router und http test Requests</t>
   </si>
 </sst>
 </file>
@@ -400,19 +406,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -423,7 +429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45363</v>
       </c>
@@ -434,7 +440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45488</v>
       </c>
@@ -445,7 +451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45379</v>
       </c>
@@ -456,7 +462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45380</v>
       </c>
@@ -465,6 +471,17 @@
       </c>
       <c r="C5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -474,18 +491,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE7B43D-064A-4B82-8DF1-53FBF226FBF2}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,7 +513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45363</v>
       </c>
@@ -507,7 +524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45488</v>
       </c>
@@ -518,7 +535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45379</v>
       </c>
@@ -529,7 +546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45380</v>
       </c>
@@ -538,6 +555,17 @@
       </c>
       <c r="C5" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -547,18 +575,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7A4CFC-292D-4A68-9CB6-60BD2C7F66B3}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -569,7 +597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45363</v>
       </c>
@@ -580,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45364</v>
       </c>
@@ -591,7 +619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45488</v>
       </c>
@@ -602,7 +630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45379</v>
       </c>
@@ -613,7 +641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45380</v>
       </c>
@@ -622,6 +650,17 @@
       </c>
       <c r="C6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>